<commit_message>
Analysis of Q12 and Q13.
</commit_message>
<xml_diff>
--- a/output/teste_qui_quadrado/qui_test_Idade_Q12.xlsx
+++ b/output/teste_qui_quadrado/qui_test_Idade_Q12.xlsx
@@ -14,13 +14,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t xml:space="preserve">statistic</t>
+    <t xml:space="preserve">Estatística</t>
   </si>
   <si>
-    <t xml:space="preserve">df</t>
+    <t xml:space="preserve">Graus de liberdade</t>
   </si>
   <si>
-    <t xml:space="preserve">p_value</t>
+    <t xml:space="preserve">Valor-p</t>
   </si>
 </sst>
 </file>

</xml_diff>